<commit_message>
updated charts with aesthetic fixes
</commit_message>
<xml_diff>
--- a/data/07_reporting/revenue_summary.xlsx
+++ b/data/07_reporting/revenue_summary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3000" yWindow="500" windowWidth="25800" windowHeight="17500" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3000" yWindow="500" windowWidth="25800" windowHeight="17500" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Revenue by FY" sheetId="1" state="visible" r:id="rId1"/>
@@ -1464,7 +1464,7 @@
   </sheetPr>
   <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+    <sheetView topLeftCell="A48" workbookViewId="0">
       <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
@@ -4587,8 +4587,8 @@
   </sheetPr>
   <dimension ref="B1:I55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4693,9 +4693,7 @@
         <f>'Revenue Data'!C3/'Revenue Data'!C2-1</f>
         <v/>
       </c>
-      <c r="E9" s="39" t="n">
-        <v>-0.06</v>
-      </c>
+      <c r="E9" s="39" t="n"/>
       <c r="F9" s="41">
         <f>'Tax Base Data'!B3/'Tax Base Data'!B2-1</f>
         <v/>
@@ -4715,9 +4713,7 @@
         <f>'Revenue Data'!C4/'Revenue Data'!C3-1</f>
         <v/>
       </c>
-      <c r="E10" s="39" t="n">
-        <v>0.0897</v>
-      </c>
+      <c r="E10" s="39" t="n"/>
       <c r="F10" s="41">
         <f>'Tax Base Data'!B4/'Tax Base Data'!B3-1</f>
         <v/>
@@ -4737,9 +4733,7 @@
         <f>'Revenue Data'!C5/'Revenue Data'!C4-1</f>
         <v/>
       </c>
-      <c r="E11" s="39" t="n">
-        <v>0.0702</v>
-      </c>
+      <c r="E11" s="39" t="n"/>
       <c r="F11" s="41">
         <f>'Tax Base Data'!B5/'Tax Base Data'!B4-1</f>
         <v/>
@@ -4759,9 +4753,7 @@
         <f>'Revenue Data'!C6/'Revenue Data'!C5-1</f>
         <v/>
       </c>
-      <c r="E12" s="39" t="n">
-        <v>0.0417</v>
-      </c>
+      <c r="E12" s="39" t="n"/>
       <c r="F12" s="41">
         <f>'Tax Base Data'!B6/'Tax Base Data'!B5-1</f>
         <v/>
@@ -4781,9 +4773,7 @@
         <f>'Revenue Data'!C7/'Revenue Data'!C6-1</f>
         <v/>
       </c>
-      <c r="E13" s="42" t="n">
-        <v>0.0363</v>
-      </c>
+      <c r="E13" s="42" t="n"/>
       <c r="F13" s="41">
         <f>'Tax Base Data'!B7/'Tax Base Data'!B6-1</f>
         <v/>
@@ -4821,9 +4811,7 @@
         <f>'Revenue Data'!C15/'Revenue Data'!C14-1</f>
         <v/>
       </c>
-      <c r="E16" s="51" t="n">
-        <v>-0.1171</v>
-      </c>
+      <c r="E16" s="51" t="n"/>
       <c r="F16" s="53">
         <f>'Tax Base Data'!D3/'Tax Base Data'!D2-1</f>
         <v/>
@@ -4843,9 +4831,7 @@
         <f>'Revenue Data'!C16/'Revenue Data'!C15-1</f>
         <v/>
       </c>
-      <c r="E17" s="39" t="n">
-        <v>0.3043</v>
-      </c>
+      <c r="E17" s="39" t="n"/>
       <c r="F17" s="53">
         <f>'Tax Base Data'!D4/'Tax Base Data'!D3-1</f>
         <v/>
@@ -4870,9 +4856,7 @@
         <f>'Revenue Data'!C17/'Revenue Data'!C16-1</f>
         <v/>
       </c>
-      <c r="E18" s="39" t="n">
-        <v>0.0415</v>
-      </c>
+      <c r="E18" s="39" t="n"/>
       <c r="F18" s="53">
         <f>'Tax Base Data'!D5/'Tax Base Data'!D4-1</f>
         <v/>
@@ -4892,9 +4876,7 @@
         <f>'Revenue Data'!C18/'Revenue Data'!C17-1</f>
         <v/>
       </c>
-      <c r="E19" s="39" t="n">
-        <v>0.0406</v>
-      </c>
+      <c r="E19" s="39" t="n"/>
       <c r="F19" s="53">
         <f>'Tax Base Data'!D6/'Tax Base Data'!D5-1</f>
         <v/>
@@ -4914,9 +4896,7 @@
         <f>'Revenue Data'!C19/'Revenue Data'!C18-1</f>
         <v/>
       </c>
-      <c r="E20" s="42" t="n">
-        <v>0.0416</v>
-      </c>
+      <c r="E20" s="42" t="n"/>
       <c r="F20" s="53">
         <f>'Tax Base Data'!D7/'Tax Base Data'!D6-1</f>
         <v/>
@@ -4954,9 +4934,7 @@
         <f>'Revenue Data'!C9/'Revenue Data'!C8-1</f>
         <v/>
       </c>
-      <c r="E23" s="39" t="n">
-        <v>-0.06270000000000001</v>
-      </c>
+      <c r="E23" s="39" t="n"/>
       <c r="F23" s="41">
         <f>'Tax Base Data'!C3/'Tax Base Data'!C2-1</f>
         <v/>
@@ -4976,9 +4954,7 @@
         <f>'Revenue Data'!C10/'Revenue Data'!C9-1</f>
         <v/>
       </c>
-      <c r="E24" s="39" t="n">
-        <v>0.0818</v>
-      </c>
+      <c r="E24" s="39" t="n"/>
       <c r="F24" s="41">
         <f>'Tax Base Data'!C4/'Tax Base Data'!C3-1</f>
         <v/>
@@ -4998,9 +4974,7 @@
         <f>'Revenue Data'!C11/'Revenue Data'!C10-1</f>
         <v/>
       </c>
-      <c r="E25" s="39" t="n">
-        <v>0.0497</v>
-      </c>
+      <c r="E25" s="39" t="n"/>
       <c r="F25" s="41">
         <f>'Tax Base Data'!C5/'Tax Base Data'!C4-1</f>
         <v/>
@@ -5020,9 +4994,7 @@
         <f>'Revenue Data'!C12/'Revenue Data'!C11-1</f>
         <v/>
       </c>
-      <c r="E26" s="39" t="n">
-        <v>0.0342</v>
-      </c>
+      <c r="E26" s="39" t="n"/>
       <c r="F26" s="41">
         <f>'Tax Base Data'!C6/'Tax Base Data'!C5-1</f>
         <v/>
@@ -5042,9 +5014,7 @@
         <f>'Revenue Data'!C13/'Revenue Data'!C12-1</f>
         <v/>
       </c>
-      <c r="E27" s="42" t="n">
-        <v>0.0326</v>
-      </c>
+      <c r="E27" s="42" t="n"/>
       <c r="F27" s="41">
         <f>'Tax Base Data'!C7/'Tax Base Data'!C6-1</f>
         <v/>
@@ -5082,9 +5052,7 @@
         <f>'Revenue Data'!C21/'Revenue Data'!C20-1</f>
         <v/>
       </c>
-      <c r="E30" s="39" t="n">
-        <v>-0.0659</v>
-      </c>
+      <c r="E30" s="39" t="n"/>
       <c r="F30" s="41">
         <f>'Tax Base Data'!G3/'Tax Base Data'!G2-1</f>
         <v/>
@@ -5104,9 +5072,7 @@
         <f>'Revenue Data'!C22/'Revenue Data'!C21-1</f>
         <v/>
       </c>
-      <c r="E31" s="39" t="n">
-        <v>0.029</v>
-      </c>
+      <c r="E31" s="39" t="n"/>
       <c r="F31" s="41">
         <f>'Tax Base Data'!G4/'Tax Base Data'!G3-1</f>
         <v/>
@@ -5126,9 +5092,7 @@
         <f>'Revenue Data'!C23/'Revenue Data'!C22-1</f>
         <v/>
       </c>
-      <c r="E32" s="39" t="n">
-        <v>0.0416</v>
-      </c>
+      <c r="E32" s="39" t="n"/>
       <c r="F32" s="41">
         <f>'Tax Base Data'!G5/'Tax Base Data'!G4-1</f>
         <v/>
@@ -5148,9 +5112,7 @@
         <f>'Revenue Data'!C24/'Revenue Data'!C23-1</f>
         <v/>
       </c>
-      <c r="E33" s="39" t="n">
-        <v>0.037</v>
-      </c>
+      <c r="E33" s="39" t="n"/>
       <c r="F33" s="41">
         <f>'Tax Base Data'!G6/'Tax Base Data'!G5-1</f>
         <v/>
@@ -5170,9 +5132,7 @@
         <f>'Revenue Data'!C25/'Revenue Data'!C24-1</f>
         <v/>
       </c>
-      <c r="E34" s="42" t="n">
-        <v>0.0376</v>
-      </c>
+      <c r="E34" s="42" t="n"/>
       <c r="F34" s="41">
         <f>'Tax Base Data'!G7/'Tax Base Data'!G6-1</f>
         <v/>
@@ -5210,9 +5170,7 @@
         <f>'Revenue Data'!C27/'Revenue Data'!C26-1</f>
         <v/>
       </c>
-      <c r="E37" s="39" t="n">
-        <v>-0.1443</v>
-      </c>
+      <c r="E37" s="39" t="n"/>
       <c r="F37" s="41">
         <f>'Tax Base Data'!H3/'Tax Base Data'!H2-1</f>
         <v/>
@@ -5232,9 +5190,7 @@
         <f>'Revenue Data'!C28/'Revenue Data'!C27-1</f>
         <v/>
       </c>
-      <c r="E38" s="39" t="n">
-        <v>0.2064</v>
-      </c>
+      <c r="E38" s="39" t="n"/>
       <c r="F38" s="41">
         <f>'Tax Base Data'!H4/'Tax Base Data'!H3-1</f>
         <v/>
@@ -5254,9 +5210,7 @@
         <f>'Revenue Data'!C29/'Revenue Data'!C28-1</f>
         <v/>
       </c>
-      <c r="E39" s="39" t="n">
-        <v>0.0326</v>
-      </c>
+      <c r="E39" s="39" t="n"/>
       <c r="F39" s="41">
         <f>'Tax Base Data'!H5/'Tax Base Data'!H4-1</f>
         <v/>
@@ -5276,9 +5230,7 @@
         <f>'Revenue Data'!C30/'Revenue Data'!C29-1</f>
         <v/>
       </c>
-      <c r="E40" s="39" t="n">
-        <v>0.027</v>
-      </c>
+      <c r="E40" s="39" t="n"/>
       <c r="F40" s="41">
         <f>'Tax Base Data'!H6/'Tax Base Data'!H5-1</f>
         <v/>
@@ -5298,9 +5250,7 @@
         <f>'Revenue Data'!C31/'Revenue Data'!C30-1</f>
         <v/>
       </c>
-      <c r="E41" s="42" t="n">
-        <v>0.0288</v>
-      </c>
+      <c r="E41" s="42" t="n"/>
       <c r="F41" s="41">
         <f>'Tax Base Data'!H7/'Tax Base Data'!H6-1</f>
         <v/>
@@ -5338,10 +5288,7 @@
         <f>'Revenue Data'!C45/'Revenue Data'!C44-1</f>
         <v/>
       </c>
-      <c r="E44" s="39">
-        <f>C44</f>
-        <v/>
-      </c>
+      <c r="E44" s="39" t="n"/>
       <c r="F44" s="41">
         <f>D44</f>
         <v/>
@@ -5361,10 +5308,7 @@
         <f>'Revenue Data'!C46/'Revenue Data'!C45-1</f>
         <v/>
       </c>
-      <c r="E45" s="39">
-        <f>C45</f>
-        <v/>
-      </c>
+      <c r="E45" s="39" t="n"/>
       <c r="F45" s="41">
         <f>D45</f>
         <v/>
@@ -5384,10 +5328,7 @@
         <f>'Revenue Data'!C47/'Revenue Data'!C46-1</f>
         <v/>
       </c>
-      <c r="E46" s="39">
-        <f>C46</f>
-        <v/>
-      </c>
+      <c r="E46" s="39" t="n"/>
       <c r="F46" s="41">
         <f>D46</f>
         <v/>
@@ -5407,10 +5348,7 @@
         <f>'Revenue Data'!C48/'Revenue Data'!C47-1</f>
         <v/>
       </c>
-      <c r="E47" s="39">
-        <f>C47</f>
-        <v/>
-      </c>
+      <c r="E47" s="39" t="n"/>
       <c r="F47" s="41">
         <f>D47</f>
         <v/>
@@ -5430,10 +5368,7 @@
         <f>'Revenue Data'!C49/'Revenue Data'!C48-1</f>
         <v/>
       </c>
-      <c r="E48" s="39">
-        <f>C48</f>
-        <v/>
-      </c>
+      <c r="E48" s="39" t="n"/>
       <c r="F48" s="41">
         <f>D48</f>
         <v/>
@@ -5471,9 +5406,7 @@
         <f>'Revenue Data'!C39/'Revenue Data'!C38-1</f>
         <v/>
       </c>
-      <c r="E51" s="39" t="n">
-        <v>-0.2383</v>
-      </c>
+      <c r="E51" s="39" t="n"/>
       <c r="F51" s="41">
         <f>'Tax Base Data'!J3/'Tax Base Data'!J2-1</f>
         <v/>
@@ -5493,9 +5426,7 @@
         <f>'Revenue Data'!C40/'Revenue Data'!C39-1</f>
         <v/>
       </c>
-      <c r="E52" s="39" t="n">
-        <v>0.3527</v>
-      </c>
+      <c r="E52" s="39" t="n"/>
       <c r="F52" s="41">
         <f>'Tax Base Data'!J4/'Tax Base Data'!J3-1</f>
         <v/>
@@ -5515,9 +5446,7 @@
         <f>'Revenue Data'!C41/'Revenue Data'!C40-1</f>
         <v/>
       </c>
-      <c r="E53" s="39" t="n">
-        <v>-0.0515</v>
-      </c>
+      <c r="E53" s="39" t="n"/>
       <c r="F53" s="41">
         <f>'Tax Base Data'!J5/'Tax Base Data'!J4-1</f>
         <v/>
@@ -5537,9 +5466,7 @@
         <f>'Revenue Data'!C42/'Revenue Data'!C41-1</f>
         <v/>
       </c>
-      <c r="E54" s="39" t="n">
-        <v>-0.0395</v>
-      </c>
+      <c r="E54" s="39" t="n"/>
       <c r="F54" s="41">
         <f>'Tax Base Data'!J6/'Tax Base Data'!J5-1</f>
         <v/>
@@ -5559,9 +5486,7 @@
         <f>'Revenue Data'!C43/'Revenue Data'!C42-1</f>
         <v/>
       </c>
-      <c r="E55" s="42" t="n">
-        <v>0.07630000000000001</v>
-      </c>
+      <c r="E55" s="42" t="n"/>
       <c r="F55" s="44">
         <f>'Tax Base Data'!J7/'Tax Base Data'!J6-1</f>
         <v/>
@@ -5597,7 +5522,7 @@
   <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView zoomScale="99" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:XFD49"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>